<commit_message>
Final draft for expected cost
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TEC\Taller de Diseño\CYAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52771FF-AC36-4E1E-B437-5816276535B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A36462B-0ECC-4D30-B585-4EEDD93E925B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1104" windowWidth="20364" windowHeight="11136" xr2:uid="{A8FCBE76-C5FC-434B-A4CE-1731A8E5FE90}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Arduino MEGA 2560</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Riel MGN9H (200 mm)</t>
   </si>
   <si>
-    <t>Timing belt</t>
-  </si>
-  <si>
     <t>tornillos</t>
   </si>
   <si>
@@ -139,12 +136,6 @@
     <t>pedazo de metal para boquilla</t>
   </si>
   <si>
-    <t>TPU</t>
-  </si>
-  <si>
-    <t>ABS</t>
-  </si>
-  <si>
     <t>Ventilador de fusor 4010</t>
   </si>
   <si>
@@ -193,15 +184,6 @@
     <t>Resorte de metal 20mm</t>
   </si>
   <si>
-    <t>Lámina de acrílico</t>
-  </si>
-  <si>
-    <t>Lámina de MDF</t>
-  </si>
-  <si>
-    <t>Lámina de vidrio</t>
-  </si>
-  <si>
     <t>rodamientos o ruedas johan</t>
   </si>
   <si>
@@ -214,9 +196,6 @@
     <t>Motor paso a paso</t>
   </si>
   <si>
-    <t>El PLA es muy débil</t>
-  </si>
-  <si>
     <t>$3,95 en MicroJPM</t>
   </si>
   <si>
@@ -224,6 +203,21 @@
   </si>
   <si>
     <t>Correa GT2 en bucle 200 mm</t>
+  </si>
+  <si>
+    <t>Correa GT2 100 cm</t>
+  </si>
+  <si>
+    <t>Lámina de acrílico 3mm (500x800)</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Panel de vidrio borosilicato (120 x 120 x 3) mm</t>
+  </si>
+  <si>
+    <t>Falta tomar en cuenta los tornillos, los insertos y las piezas correspondientes a los ensambles de Johan.</t>
   </si>
 </sst>
 </file>
@@ -233,7 +227,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="165" formatCode="_-[$₡-140A]* #,##0.00_-;\-[$₡-140A]* #,##0.00_-;_-[$₡-140A]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_([$$-409]* #,##0.000000_);_([$$-409]* \(#,##0.000000\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.000000_);_([$$-409]* \(#,##0.000000\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -716,7 +710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -903,8 +897,8 @@
     <v>USD</v>
     <v>516.08000000000004</v>
     <v>Currency Pair</v>
-    <v>45534.671215277776</v>
-    <v>521.32000000000005</v>
+    <v>45534.807905092595</v>
+    <v>521</v>
     <v>US Dollar/Costa Rica Colon FX Spot Rate</v>
     <v>515.95000000000005</v>
     <v>515.95000000000005</v>
@@ -933,9 +927,9 @@
     <v>5.2220000000000001E-4</v>
     <v>USD</v>
     <v>CRC</v>
-    <v>1.918E-3</v>
+    <v>1.9189999999999999E-3</v>
     <v>Currency Pair</v>
-    <v>45534.671215277776</v>
+    <v>45534.807905092595</v>
     <v>1.9380000000000001E-3</v>
     <v>Costa Rica Colon/US Dollar FX Cross Rate</v>
     <v>1.915E-3</v>
@@ -1460,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9C911C-6DDC-476A-A77C-DCF06B8F150E}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1490,13 +1484,13 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1515,7 +1509,7 @@
         <v>34.950000000000003</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -1544,7 +1538,7 @@
         <v>17.95</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J3" t="e" vm="2">
         <v>#VALUE!</v>
@@ -1556,7 +1550,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1572,7 +1566,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1588,7 +1582,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1602,7 +1596,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -1670,7 +1664,7 @@
         <v>34.75</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1685,11 +1679,11 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="1">
-        <f t="shared" ref="E11:E36" si="1">C11*B11</f>
+        <f t="shared" ref="E11:E33" si="1">C11*B11</f>
         <v>39.950000000000003</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
@@ -1726,7 +1720,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1740,12 +1734,12 @@
         <v>4.99</v>
       </c>
       <c r="F14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1761,7 +1755,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -1775,19 +1769,25 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>41</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5.99</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>23.96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1801,9 +1801,9 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1">
         <f>8.99/100</f>
@@ -1815,9 +1815,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1834,12 +1834,12 @@
         <v>0.68975999999999993</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1856,12 +1856,12 @@
         <v>2.8548399999999998</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -1869,14 +1869,15 @@
       <c r="C22" s="1">
         <v>2.4900000000000002</v>
       </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="1">
         <f t="shared" si="1"/>
         <v>9.9600000000000009</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B23">
         <v>16</v>
@@ -1885,17 +1886,18 @@
         <f>6/4</f>
         <v>1.5</v>
       </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="1">
         <f>C23*B23</f>
         <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1903,164 +1905,168 @@
       <c r="C24" s="1">
         <v>39.950000000000003</v>
       </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="1">
         <f t="shared" si="1"/>
         <v>39.950000000000003</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <f>D26*K3</f>
+        <v>12.453999999999999</v>
+      </c>
+      <c r="D26" s="2">
+        <v>6500</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.453999999999999</v>
       </c>
       <c r="F26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>38</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <f>28.69</f>
+        <v>28.69</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>28.69</v>
       </c>
       <c r="F27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>39</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>18</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30" s="1">
+        <f>9.99/10</f>
+        <v>0.999</v>
+      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15.984</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="B31">
-        <v>16</v>
-      </c>
-      <c r="C31" s="1">
-        <f>9.99/10</f>
-        <v>0.999</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="1">
         <f t="shared" si="1"/>
-        <v>15.984</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>40</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1">
+        <v>4.99</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>14.97</v>
+      </c>
+      <c r="F32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="1">
-        <v>4.99</v>
-      </c>
+        <f>3/40</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="1">
         <f t="shared" si="1"/>
-        <v>14.97</v>
-      </c>
-      <c r="F33" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33" t="s">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="5">
+        <f>SUM(E2:E33)</f>
+        <v>595.55259999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G35" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-      <c r="C36" s="1">
-        <f>3/40</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="E36" s="1">
-        <f t="shared" si="1"/>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="5">
-        <f>SUM(E2:E36)</f>
-        <v>530.44859999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de costos de materia prima
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TEC\Taller de Diseño\CYAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC2F6C9-A3CC-4F76-B7A0-D782FCCBDEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D99131-FFAD-4BFA-B8FD-850FA79FB4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1104" windowWidth="20364" windowHeight="11136" xr2:uid="{A8FCBE76-C5FC-434B-A4CE-1731A8E5FE90}"/>
+    <workbookView xWindow="1152" yWindow="1104" windowWidth="20316" windowHeight="11136" xr2:uid="{A8FCBE76-C5FC-434B-A4CE-1731A8E5FE90}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Arduino MEGA 2560</t>
   </si>
@@ -127,15 +127,6 @@
     <t>Riel MGN9H (200 mm)</t>
   </si>
   <si>
-    <t>tornillos</t>
-  </si>
-  <si>
-    <t>pedazo de metal para husillo</t>
-  </si>
-  <si>
-    <t>pedazo de metal para boquilla</t>
-  </si>
-  <si>
     <t>Ventilador de fusor 4010</t>
   </si>
   <si>
@@ -160,9 +151,6 @@
     <t>Niple cromado 1/2"</t>
   </si>
   <si>
-    <t>Zip-Tie</t>
-  </si>
-  <si>
     <t>Polea 20T</t>
   </si>
   <si>
@@ -199,31 +187,31 @@
     <t>Lámina de acrílico 3mm (500x800)</t>
   </si>
   <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>Panel de vidrio borosilicato (120 x 120 x 3) mm</t>
-  </si>
-  <si>
     <t>Arandela - Calidad A - DIN 125</t>
   </si>
   <si>
     <t>Roles para impresoras 3D</t>
   </si>
   <si>
-    <t>Tornillo con cabeza hueca (M3 x 30)</t>
-  </si>
-  <si>
-    <t>Tornillo con cabeza hueca (M5 x 25)</t>
-  </si>
-  <si>
-    <t>Tornillo con cabeza hueca (M2 x 8)</t>
-  </si>
-  <si>
-    <t>tuercas</t>
-  </si>
-  <si>
-    <t>tuercas nylon</t>
+    <t>Zip-Ties</t>
+  </si>
+  <si>
+    <t>Tornillos</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Rodamientos de bolas F625</t>
+  </si>
+  <si>
+    <t>CRCibernética</t>
+  </si>
+  <si>
+    <t>Universal Tornillos</t>
+  </si>
+  <si>
+    <t>Insertos roscados M5</t>
   </si>
 </sst>
 </file>
@@ -712,7 +700,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -721,6 +709,12 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1460,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9C911C-6DDC-476A-A77C-DCF06B8F150E}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1490,13 +1484,13 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1511,11 +1505,11 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="1">
-        <f t="shared" ref="E2:E9" si="0">C2*B2</f>
+        <f t="shared" ref="E2:E8" si="0">C2*B2</f>
         <v>34.950000000000003</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -1524,7 +1518,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="K2" s="2" cm="1">
-        <f t="array" ref="K2">_FV(J2,"Price")</f>
+        <f t="array" aca="1" ref="K2" ca="1">_FV(J2,"Price")</f>
         <v>516.5</v>
       </c>
     </row>
@@ -1544,22 +1538,22 @@
         <v>17.95</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J3" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="K3" s="3" cm="1">
-        <f t="array" ref="K3">_FV(J3,"Price")</f>
+        <f t="array" aca="1" ref="K3" ca="1">_FV(J3,"Price")</f>
         <v>1.913E-3</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>21</v>
@@ -1567,294 +1561,294 @@
       <c r="D4" s="2"/>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>105</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>19.5</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>19.5</v>
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>6.99</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
+        <v>13.98</v>
+      </c>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>6.99</v>
+        <v>8.49</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>13.98</v>
-      </c>
-      <c r="N7" s="2"/>
+        <v>25.47</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" s="1">
-        <v>8.49</v>
+        <v>8.99</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>25.47</v>
+        <v>26.97</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
-        <v>8.99</v>
+        <v>6.95</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>26.97</v>
+        <f>C9*B9</f>
+        <v>34.75</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>6.95</v>
+        <v>39.950000000000003</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="1">
-        <f>C10*B10</f>
-        <v>34.75</v>
+        <f t="shared" ref="E10:E30" si="1">C10*B10</f>
+        <v>39.950000000000003</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>39.950000000000003</v>
+        <v>29.95</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="1">
-        <f t="shared" ref="E11:E38" si="1">C11*B11</f>
-        <v>39.950000000000003</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>59.9</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>29.95</v>
+        <v>16.5</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="1">
         <f t="shared" si="1"/>
-        <v>59.9</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>16.5</v>
+        <v>4.99</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="1">
         <f t="shared" si="1"/>
-        <v>16.5</v>
+        <v>4.99</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>4.99</v>
+        <v>6.5</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="1">
         <f t="shared" si="1"/>
-        <v>4.99</v>
-      </c>
-      <c r="F14" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" s="1">
-        <v>6.5</v>
+        <v>5.99</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>11.98</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>5.99</v>
+        <v>3.99</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="1">
         <f t="shared" si="1"/>
-        <v>23.96</v>
+        <v>3.99</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1">
-        <v>3.99</v>
+        <f>8.99/100</f>
+        <v>8.9900000000000008E-2</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="1">
         <f t="shared" si="1"/>
-        <v>3.99</v>
+        <v>0.89900000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>1</v>
-      </c>
-      <c r="C18" s="1">
-        <f>8.99/100</f>
-        <v>8.9900000000000008E-2</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="1">
         <f t="shared" si="1"/>
-        <v>8.9900000000000008E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="1">
-        <f>D19*K3</f>
+        <f ca="1">D19*K3</f>
         <v>0.68867999999999996</v>
       </c>
       <c r="D19" s="2">
         <v>360</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>0.68867999999999996</v>
       </c>
       <c r="F19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="1">
-        <f>D20*K3</f>
+        <f ca="1">D20*K3</f>
         <v>2.8503699999999998</v>
       </c>
       <c r="D20" s="2">
         <v>1490</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ca="1" si="1"/>
         <v>2.8503699999999998</v>
       </c>
       <c r="F20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -1870,7 +1864,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1884,12 +1878,12 @@
         <v>39.950000000000003</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>16</v>
@@ -1905,7 +1899,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -1920,204 +1914,126 @@
         <v>6.8999999999999995</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>38</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f ca="1">6700/K2</f>
+        <v>12.971926427879961</v>
+      </c>
+      <c r="F25" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B26">
-        <v>8</v>
-      </c>
-      <c r="D26" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <f ca="1">D26*K3</f>
+        <v>12.4345</v>
+      </c>
+      <c r="D26" s="2">
+        <v>6500</v>
+      </c>
       <c r="E26" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>12.4345</v>
+      </c>
+      <c r="F26" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="C27" s="1">
+        <f>9.99/10</f>
+        <v>0.999</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15.984</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2.99</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.98</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3.95</v>
       </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1">
+        <f t="shared" si="1"/>
+        <v>11.850000000000001</v>
+      </c>
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="1">
-        <f>D32*K3</f>
-        <v>12.4345</v>
-      </c>
-      <c r="D32" s="2">
-        <v>6500</v>
-      </c>
-      <c r="E32" s="1">
-        <f t="shared" si="1"/>
-        <v>12.4345</v>
-      </c>
-      <c r="F32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1">
-        <f>28.69</f>
-        <v>28.69</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="1">
-        <f t="shared" si="1"/>
-        <v>28.69</v>
-      </c>
-      <c r="F33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36">
-        <v>16</v>
-      </c>
-      <c r="C36" s="1">
-        <f>9.99/10</f>
-        <v>0.999</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="1">
-        <f t="shared" si="1"/>
-        <v>15.984</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="C37" s="1">
-        <v>3.95</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="1">
-        <f t="shared" si="1"/>
-        <v>11.850000000000001</v>
-      </c>
-      <c r="F37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38">
-        <v>2</v>
-      </c>
-      <c r="C38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1">
         <f>3/40</f>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="1">
+      <c r="D30" s="2"/>
+      <c r="E30" s="1">
         <f t="shared" si="1"/>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="5">
-        <f>SUM(E2:E38)</f>
-        <v>552.04744999999991</v>
+      <c r="E31" s="5">
+        <f ca="1">SUM(E2:E30)</f>
+        <v>533.01347642787994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted deck panel, updated BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TEC\Taller de Diseño\CYAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CYAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D99131-FFAD-4BFA-B8FD-850FA79FB4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7411BA81-9765-4650-9F38-1A3178BF0C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1104" windowWidth="20316" windowHeight="11136" xr2:uid="{A8FCBE76-C5FC-434B-A4CE-1731A8E5FE90}"/>
+    <workbookView xWindow="3240" yWindow="3240" windowWidth="16680" windowHeight="11295" xr2:uid="{A8FCBE76-C5FC-434B-A4CE-1731A8E5FE90}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -717,48 +717,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -889,20 +889,20 @@
     <v>3</v>
     <v>Finance</v>
     <v>4</v>
-    <v>538.04999999999995</v>
+    <v>532.14</v>
     <v>497</v>
-    <v>0.66</v>
-    <v>1.2790000000000002E-3</v>
+    <v>0</v>
+    <v>0</v>
     <v>CRC</v>
     <v>USD</v>
-    <v>517</v>
+    <v>507.75</v>
     <v>Currency Pair</v>
-    <v>45559.697893518518</v>
-    <v>521.75</v>
+    <v>45610.003807870373</v>
+    <v>513.9</v>
     <v>US Dollar/Costa Rica Colon FX Spot Rate</v>
-    <v>515.84</v>
-    <v>515.84</v>
-    <v>516.5</v>
+    <v>507.75</v>
+    <v>507.75</v>
+    <v>507.75</v>
     <v>USDCRC</v>
     <v>USD/CRC</v>
   </rv>
@@ -922,19 +922,19 @@
     <v>Finance</v>
     <v>4</v>
     <v>1.99E-3</v>
-    <v>1.8400000000000001E-3</v>
-    <v>-3.0000000000000001E-6</v>
-    <v>-1.5659999999999999E-3</v>
+    <v>1.8500000000000001E-3</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>CRC</v>
-    <v>1.9170000000000001E-3</v>
+    <v>1.946E-3</v>
     <v>Currency Pair</v>
-    <v>45559.697893518518</v>
-    <v>1.934E-3</v>
+    <v>45610.003807870373</v>
+    <v>1.9689999999999998E-3</v>
     <v>Costa Rica Colon/US Dollar FX Cross Rate</v>
-    <v>1.916E-3</v>
-    <v>1.916E-3</v>
-    <v>1.913E-3</v>
+    <v>1.946E-3</v>
+    <v>1.946E-3</v>
+    <v>1.946E-3</v>
     <v>CRCUSD</v>
     <v>CRC/USD</v>
   </rv>
@@ -1138,7 +1138,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1456,21 +1456,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9C911C-6DDC-476A-A77C-DCF06B8F150E}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E31" sqref="A1:E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1519,10 +1519,10 @@
       </c>
       <c r="K2" s="2" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">_FV(J2,"Price")</f>
-        <v>516.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>507.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1545,10 +1545,10 @@
       </c>
       <c r="K3" s="3" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">_FV(J3,"Price")</f>
-        <v>1.913E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1.946E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>25.47</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>26.97</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>59.9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>11.98</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1789,20 +1789,23 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
       <c r="B18">
         <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.26</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1811,20 +1814,20 @@
       </c>
       <c r="C19" s="1">
         <f ca="1">D19*K3</f>
-        <v>0.68867999999999996</v>
+        <v>0.70055999999999996</v>
       </c>
       <c r="D19" s="2">
         <v>360</v>
       </c>
       <c r="E19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0.68867999999999996</v>
+        <v>0.70055999999999996</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1833,20 +1836,20 @@
       </c>
       <c r="C20" s="1">
         <f ca="1">D20*K3</f>
-        <v>2.8503699999999998</v>
+        <v>2.89954</v>
       </c>
       <c r="D20" s="2">
         <v>1490</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8503699999999998</v>
+        <v>2.89954</v>
       </c>
       <c r="F20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1862,7 +1865,7 @@
         <v>9.9600000000000009</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1881,7 +1884,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1897,7 +1900,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1930,13 +1933,13 @@
       <c r="D25" s="2"/>
       <c r="E25" s="1">
         <f ca="1">6700/K2</f>
-        <v>12.971926427879961</v>
+        <v>13.195470211718366</v>
       </c>
       <c r="F25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1945,20 +1948,20 @@
       </c>
       <c r="C26" s="1">
         <f ca="1">D26*K3</f>
-        <v>12.4345</v>
+        <v>12.649000000000001</v>
       </c>
       <c r="D26" s="2">
         <v>6500</v>
       </c>
       <c r="E26" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>12.4345</v>
+        <v>12.649000000000001</v>
       </c>
       <c r="F26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1975,7 +1978,7 @@
         <v>15.984</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>5.98</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2010,7 +2013,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -2027,13 +2030,13 @@
         <v>0.52500000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="5">
         <f ca="1">SUM(E2:E30)</f>
-        <v>533.01347642787994</v>
+        <v>533.77257021171829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>